<commit_message>
Created Several workflows that go up until the min max median step
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/FrameworkTemplates/REFramework/VB/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndreiHandrau\Documents\GitHub\Orange_PoC\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1E2088-B8D7-4CDE-8ED2-FF3F330F06B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10248" yWindow="17508" windowWidth="21252" windowHeight="9444" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -160,6 +160,18 @@
   </si>
   <si>
     <t>ProcessABCQueue</t>
+  </si>
+  <si>
+    <t>inputFilePath</t>
+  </si>
+  <si>
+    <t>Data\Input\stat_plata_extins.xlsx</t>
+  </si>
+  <si>
+    <t>neededRows</t>
+  </si>
+  <si>
+    <t>CUI;DEPARTAMENT;SUBDEPARTAMENT;FUNCTIE;TARIFAR INCADRARE;REALIZAT SUPLIMENTAR;ORE DE NOAPTE;SPOR DE NOAPTE;PARTE VARIABILA NET;PRIMA DETASARE NET;NET PRIMA DE POST NET;PRIMA DE POST;PRIMA DE POST BRUT;PRIMA EXCEPTIONALA NET;PRIMA EXPATRIERE NET;PRIMA INTERIMAT NET;PRIMA MOBILITATE NET;PRIMA DETASARE BRUT;PRIMA OBISNUITA NETA;Regularizari Net;BONUS;PRIMA BRUTA ONCALL;PRIMA BRUTA OVERTIME;BENEFICIU IN NATURA;BRUT PT IMPOZITARE;BAZA CALCUL SOMAJ 1;BAZA CALCUL CAS;BAZA SANATATE;VENIT NET PT IMPOZITARE;BAZA PT IMPOZITARE;BRUT TICHETE MASA;BRUT TOTAL TICHETE;NET;CONTRIBUTIE SCHEMA PENSII;BRUT DIURNA DELEGATIE</t>
   </si>
 </sst>
 </file>
@@ -177,6 +189,7 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="6"/>
@@ -537,16 +550,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="2" max="2" width="93.1796875" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -594,7 +607,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -604,7 +617,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -617,9 +630,23 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="299" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1623,12 +1650,12 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1665,7 +1692,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1676,7 +1703,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1790,7 +1817,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2786,12 +2813,12 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.90625" customWidth="1"/>
+    <col min="2" max="2" width="30.08984375" customWidth="1"/>
+    <col min="3" max="3" width="60.36328125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Final Commit. Everything appears to be working as expected
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndreiHandrau\Documents\GitHub\Orange_PoC\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EB1D5D-40DE-4CD2-BFCF-21632D6F0102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D319BFA-C8C8-4C15-82C6-3380441C3C56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="74">
   <si>
     <t>Name</t>
   </si>
@@ -178,6 +178,75 @@
   </si>
   <si>
     <t>Departament;Subdepartament;FUNCTIE</t>
+  </si>
+  <si>
+    <t>Data\Output\MinMaxMed.xlsx</t>
+  </si>
+  <si>
+    <t>Data\Output\companiiGraph.xlsx</t>
+  </si>
+  <si>
+    <t>companiiGraphPath</t>
+  </si>
+  <si>
+    <t>pdfPath</t>
+  </si>
+  <si>
+    <t>Data\Output\PDF_COMPANII\</t>
+  </si>
+  <si>
+    <t>centralizatorPath</t>
+  </si>
+  <si>
+    <t>zipPath</t>
+  </si>
+  <si>
+    <t>Data\Output\HANDRAU</t>
+  </si>
+  <si>
+    <t>itemURL</t>
+  </si>
+  <si>
+    <t>sharepointSite</t>
+  </si>
+  <si>
+    <t>libName</t>
+  </si>
+  <si>
+    <t>itemURLSharepoint</t>
+  </si>
+  <si>
+    <t>itemURLZIP</t>
+  </si>
+  <si>
+    <t>devs\'Shared Folder'\HandrauAndrei</t>
+  </si>
+  <si>
+    <t>Documente</t>
+  </si>
+  <si>
+    <t>companiiPath</t>
+  </si>
+  <si>
+    <t>Data\Output\Companii.xlsx</t>
+  </si>
+  <si>
+    <t>Documente partajate\devs\'Shared Folder'\HandrauAndrei</t>
+  </si>
+  <si>
+    <t>emailReceiver</t>
+  </si>
+  <si>
+    <t>ionut.onea@fwfcompany.com</t>
+  </si>
+  <si>
+    <t>The Process Executed Successfully</t>
+  </si>
+  <si>
+    <t>emailSubject</t>
+  </si>
+  <si>
+    <t>https://futureworkforcecompany.sharepoint.com/sites/dreamteam/</t>
   </si>
 </sst>
 </file>
@@ -230,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -240,6 +309,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -644,44 +715,125 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="299" customHeight="1">
-      <c r="A10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>48</v>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="299" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
         <v>49</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B16" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1648,6 +1800,10 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
+    <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="1001" ht="14.25" customHeight="1"/>
+    <row r="1002" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>